<commit_message>
added metrics and added streamlit for frontend UI
</commit_message>
<xml_diff>
--- a/example/Data/Golden_data_sample.xlsx
+++ b/example/Data/Golden_data_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michelingroup-my.sharepoint.com/personal/ankit_zade_michelin_com/Documents/Ankit/Projects/Initiatives/LLM/LLMInspector/Open Source sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michelingroup-my.sharepoint.com/personal/shraddha_pawar_michelin_com/Documents/Documents/LLMInspector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{27BACF95-4801-46D1-B762-FFBE01D67348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35672010-465F-481D-B8B5-2C82AC478AE6}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{27BACF95-4801-46D1-B762-FFBE01D67348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D059BE8C-C0B6-4AC8-8232-E8A90B0C85E2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FEE1D6B1-3CC4-4256-96DE-352312A230E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEE1D6B1-3CC4-4256-96DE-352312A230E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>input_prompt</t>
-  </si>
-  <si>
-    <t>expected_response</t>
-  </si>
-  <si>
     <t>{greeting}, how are you?</t>
   </si>
   <si>
@@ -427,13 +421,19 @@
   </si>
   <si>
     <t xml:space="preserve">I'm sorry to hear that you're feeling sad today. It's completely okay to have days when you're not feeling your best. If you'd like, we can talk about what's been on your mind, or if you prefer, I can offer some suggestions for activities that might help lift your spirits. </t>
+  </si>
+  <si>
+    <t>UserInput</t>
+  </si>
+  <si>
+    <t>Expected_Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,13 +493,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -841,248 +838,251 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3B68F2-463F-4F1D-A20A-44A54C4470C9}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="8"/>
-    <col min="2" max="2" width="63.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="8.7109375" style="7"/>
+    <col min="2" max="2" width="63.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29.1">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.5">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.1">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57.95">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29.1">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="29.1">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="5" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="29.1">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="29.1">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="57.95">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="57.95">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="29.1">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="9" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="57.95">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>